<commit_message>
Add DUO code to the xlsx form.
</commit_message>
<xml_diff>
--- a/submission_pack/EGA_policy.xlsx
+++ b/submission_pack/EGA_policy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zl/work/ega-submissions/submission_pack/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BBB968-DA03-6547-94B0-C9B2AAB938BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573CC950-25A5-D248-B7CE-64377FEBDAD9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44260" yWindow="480" windowWidth="22940" windowHeight="20900" activeTab="5" xr2:uid="{E1C644DA-B0F1-2040-B5CE-06EB24BA1ACA}"/>
+    <workbookView xWindow="44260" yWindow="480" windowWidth="22940" windowHeight="20900" activeTab="7" xr2:uid="{E1C644DA-B0F1-2040-B5CE-06EB24BA1ACA}"/>
   </bookViews>
   <sheets>
     <sheet name="INFO DAC" sheetId="3" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="Contact" sheetId="7" r:id="rId4"/>
     <sheet name="INFO Policy" sheetId="1" r:id="rId5"/>
     <sheet name="Policy" sheetId="2" r:id="rId6"/>
+    <sheet name="INFO DUO" sheetId="8" r:id="rId7"/>
+    <sheet name="DUO" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="40">
   <si>
     <t>Notes</t>
   </si>
@@ -123,6 +125,33 @@
   </si>
   <si>
     <t>Policy_links</t>
+  </si>
+  <si>
+    <t>DB</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Modifiers</t>
+  </si>
+  <si>
+    <t>The ontology database name for data use. Default is DUO.</t>
+  </si>
+  <si>
+    <t>The ID of the ontology in the database.</t>
+  </si>
+  <si>
+    <t>The version of this ontology.</t>
+  </si>
+  <si>
+    <t>The alias for the policy that this data use code should be applied to.</t>
+  </si>
+  <si>
+    <t>If a data use term is applied to a specific disease, please provide the ontological terms for such disease, separated by ",".</t>
   </si>
 </sst>
 </file>
@@ -698,7 +727,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A8"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -780,7 +809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4926A516-E8E5-DC43-9C9B-2A61C14EC092}">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -812,4 +841,103 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AFA2140-E969-8340-92B9-F2B771E79EDB}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="2" max="2" width="101.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5728E758-7572-5445-B3C5-A1FF184820EE}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add changes suggested in reviews.
</commit_message>
<xml_diff>
--- a/submission_pack/EGA_policy.xlsx
+++ b/submission_pack/EGA_policy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zl/work/ega-submissions/submission_pack/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573CC950-25A5-D248-B7CE-64377FEBDAD9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF9A7F6C-A391-FA47-B506-4F4D5612A501}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44260" yWindow="480" windowWidth="22940" windowHeight="20900" activeTab="7" xr2:uid="{E1C644DA-B0F1-2040-B5CE-06EB24BA1ACA}"/>
+    <workbookView xWindow="35160" yWindow="1820" windowWidth="30180" windowHeight="18860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INFO DAC" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="INFO DUO" sheetId="8" r:id="rId7"/>
     <sheet name="DUO" sheetId="9" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="55">
   <si>
     <t>Notes</t>
   </si>
@@ -67,15 +67,6 @@
     <t>Main_contact</t>
   </si>
   <si>
-    <t>"1" if this contact person is the main contact, otherwise "0".</t>
-  </si>
-  <si>
-    <t>The DAC this contact person is for.</t>
-  </si>
-  <si>
-    <t>The alias for this DAC (must be unique in this sheet).</t>
-  </si>
-  <si>
     <t>Name of the contact person.</t>
   </si>
   <si>
@@ -103,15 +94,9 @@
     <t>Policy_alias</t>
   </si>
   <si>
-    <t>The alias for this policy.</t>
-  </si>
-  <si>
     <t>Short text that can be used to call out data access policies in searches or in displays.</t>
   </si>
   <si>
-    <t>The alias for the DAC that this policy is associated with.</t>
-  </si>
-  <si>
     <t>Policy_text</t>
   </si>
   <si>
@@ -124,9 +109,6 @@
     <t>File containing the policy text. (Must use either Policy_text or Policy_file field, not both)</t>
   </si>
   <si>
-    <t>Policy_links</t>
-  </si>
-  <si>
     <t>DB</t>
   </si>
   <si>
@@ -145,13 +127,76 @@
     <t>The ID of the ontology in the database.</t>
   </si>
   <si>
-    <t>The version of this ontology.</t>
-  </si>
-  <si>
-    <t>The alias for the policy that this data use code should be applied to.</t>
-  </si>
-  <si>
-    <t>If a data use term is applied to a specific disease, please provide the ontological terms for such disease, separated by ",".</t>
+    <t>"1" if this contact person is the main contact, otherwise "0". This value defaults to 1.</t>
+  </si>
+  <si>
+    <t>Policy_link</t>
+  </si>
+  <si>
+    <t>Link(s) the the policy and related resources, in ';'? separated list</t>
+  </si>
+  <si>
+    <t>If a data use term is applied to a specific disease, please provide the ontological terms for such disease, separated by "," ( e.g. for HPO this would be HPO:0001234 ).</t>
+  </si>
+  <si>
+    <t>Initials of the middle name of the contact person.</t>
+  </si>
+  <si>
+    <t>Middle_initials</t>
+  </si>
+  <si>
+    <t>Surname</t>
+  </si>
+  <si>
+    <t>Title of contact person.</t>
+  </si>
+  <si>
+    <t>Surname of the contact person.</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Address of the contact person.</t>
+  </si>
+  <si>
+    <t>The DAC this contact person is for. Either this or or DAC_ID must be submitted.</t>
+  </si>
+  <si>
+    <t>The DAC EGA DAC accession this contact person is for. Either this or DAC_alias must be submitted.</t>
+  </si>
+  <si>
+    <t>The alias for the DAC that this policy is administered by. Either this or or DAC_ID must be submitted.</t>
+  </si>
+  <si>
+    <t>The ID of the DAC this policy is administered by. Either this or or DAC_alias must be submitted.</t>
+  </si>
+  <si>
+    <t>The version of this ontology. Defaults to the latest version in the case of DUO</t>
+  </si>
+  <si>
+    <t>Policy_ID</t>
+  </si>
+  <si>
+    <t>The EGA accession for the policy that this data use code should be applied to. Either this or the Policy_alias must be given.</t>
+  </si>
+  <si>
+    <t>The alias for the policy that this data use code should be applied to. Either this or the Policy_alias must be given.</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">URL referencing the URL of the Ontology. </t>
+  </si>
+  <si>
+    <t>The EGA DAC accession. Either this or or DAC_alias must be submitted.</t>
+  </si>
+  <si>
+    <t>The alias for this DAC. Either this or or DAC_ID must be submitted.</t>
+  </si>
+  <si>
+    <t>The alias for this policy. Either this or the Policy_ID must be given.</t>
   </si>
 </sst>
 </file>
@@ -187,12 +232,24 @@
       <name val="Calibri (Body)_x0000_"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -207,11 +264,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -525,14 +587,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC8BD133-06CB-7C4C-B543-6793C3CCBBC2}">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="20.33203125" customWidth="1"/>
     <col min="2" max="2" width="67.6640625" customWidth="1"/>
@@ -547,35 +609,43 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="B3" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -584,27 +654,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F131916D-3C76-7048-A95F-2D358F707E88}">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -613,17 +686,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF595908-C821-F948-8537-FB6D0483D4F8}">
-  <dimension ref="A1:B7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="50.33203125" customWidth="1"/>
+    <col min="2" max="2" width="82.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -636,84 +709,146 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="2" t="s">
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+      <c r="B10" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
-        <v>11</v>
+      <c r="B12" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46418874-9BCC-C74D-B03C-78038D54D280}">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
+  <cols>
+    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:11">
       <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -723,17 +858,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34BEE92-34DC-214A-A468-222E494F7923}">
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="19.5" customWidth="1"/>
-    <col min="2" max="2" width="74.6640625" customWidth="1"/>
+    <col min="2" max="2" width="110.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -745,97 +880,120 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B8" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" t="s">
-        <v>21</v>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4926A516-E8E5-DC43-9C9B-2A61C14EC092}">
-  <dimension ref="A1:G1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" t="s">
-        <v>20</v>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -844,17 +1002,17 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AFA2140-E969-8340-92B9-F2B771E79EDB}">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="15.1640625" customWidth="1"/>
-    <col min="2" max="2" width="101.5" customWidth="1"/>
+    <col min="2" max="2" width="138.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -867,42 +1025,58 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>38</v>
+      <c r="A5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" t="s">
+      <c r="A6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
         <v>34</v>
       </c>
-      <c r="B6" t="s">
-        <v>39</v>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -911,30 +1085,34 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5728E758-7572-5445-B3C5-A1FF184820EE}">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" t="s">
-        <v>34</v>
+        <v>27</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove 'center_name' from DAC and Policy tabs
</commit_message>
<xml_diff>
--- a/submission_pack/EGA_policy.xlsx
+++ b/submission_pack/EGA_policy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zl/work/ega-submissions/submission_pack/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF9A7F6C-A391-FA47-B506-4F4D5612A501}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB99871-79C8-9642-B1A1-1C9097629477}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35160" yWindow="1820" windowWidth="30180" windowHeight="18860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35160" yWindow="1820" windowWidth="30180" windowHeight="18860" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INFO DAC" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="54">
   <si>
     <t>Notes</t>
   </si>
@@ -86,9 +86,6 @@
   </si>
   <si>
     <t>Center_name</t>
-  </si>
-  <si>
-    <t>The center name.</t>
   </si>
   <si>
     <t>Policy_alias</t>
@@ -588,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
@@ -613,7 +610,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -621,7 +618,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -638,14 +635,6 @@
       </c>
       <c r="B5" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -712,7 +701,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -725,18 +714,18 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -749,10 +738,10 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="s">
         <v>40</v>
-      </c>
-      <c r="B7" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -768,7 +757,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -776,7 +765,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -792,7 +781,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -825,16 +814,16 @@
         <v>6</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>8</v>
@@ -859,10 +848,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
@@ -881,18 +870,18 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>47</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -900,7 +889,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -908,7 +897,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -916,39 +905,31 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
         <v>32</v>
-      </c>
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -969,10 +950,10 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>3</v>
@@ -984,13 +965,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>22</v>
-      </c>
       <c r="H1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I1" t="s">
         <v>17</v>
@@ -1005,8 +986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
@@ -1025,58 +1006,58 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" t="s">
         <v>50</v>
-      </c>
-      <c r="B8" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1094,25 +1075,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" t="s">
-        <v>28</v>
-      </c>
       <c r="G1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>